<commit_message>
Additional studies to check
</commit_message>
<xml_diff>
--- a/conceptual paper/study summary.xlsx
+++ b/conceptual paper/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="20740" yWindow="2040" windowWidth="24960" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all studies" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1634" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="428">
   <si>
     <t>define match</t>
   </si>
@@ -1335,6 +1335,24 @@
   </si>
   <si>
     <t>Visser et al. 1998; Stenseth</t>
+  </si>
+  <si>
+    <t>invertebrate (insect (family level)</t>
+  </si>
+  <si>
+    <t>(5) Saino, N., Ambrosini, R., Rubolini, D., von Hardenberg, J., Provenzale, A., Huppop, K. et al. (2011) Climate warming, ecological mismatch at arrival and population decline in migratory birds. Proceedings of the Royal Society of London B, 278, 835–842.’’</t>
+  </si>
+  <si>
+    <t>(6) Samplonius, J.M., Kappers, E.F., Brands, S. and Both, C., 2016. Phenological mismatch and ontogenetic diet shifts interactively affect offspring condition in a passerine. Journal of Animal Ecology, 85(5), pp.1255-1264.</t>
+  </si>
+  <si>
+    <t>(7) Knell, R.J. and Thackeray, S.J., 2016. Voltinism and resilience to climate-induced phenological mismatch. Climatic change, 137(3-4), pp.525-539.</t>
+  </si>
+  <si>
+    <t>(8) Abarca M. 2015 Warming effects hatching time and early season survival</t>
+  </si>
+  <si>
+    <t>Senner, N.R., Stager, M. and Sandercock, B.K., 2017. Ecological mismatches are moderated by local conditions for two populations of a long‐distance migratory bird. Oikos, 126(1), pp.61-72.</t>
   </si>
 </sst>
 </file>
@@ -3340,11 +3358,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3847,6 +3865,31 @@
     <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -3865,8 +3908,8 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1048576"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7472,30 +7515,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L28" sqref="L28"/>
+    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.5" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18" style="4" customWidth="1"/>
-    <col min="9" max="9" width="26.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="19.1640625" style="4" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5" style="4" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="19.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18" style="4" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1">
+    <row r="1" spans="1:13" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -7503,1167 +7545,1065 @@
         <v>137</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="5"/>
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>191</v>
+        <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>54</v>
+        <v>265</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>192</v>
+        <v>266</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
-        <v>301</v>
+        <v>176</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>294</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>297</v>
+        <v>172</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>301</v>
+        <v>58</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>178</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>295</v>
+        <v>185</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>118</v>
+        <v>285</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>119</v>
+        <v>63</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>120</v>
+        <v>286</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="J4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="K6" s="32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>386</v>
-      </c>
-      <c r="G5" s="4" t="s">
+    <row r="7" spans="1:13">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="165">
+      <c r="A8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="I8" s="29" t="s">
         <v>253</v>
       </c>
-      <c r="H5" s="16" t="s">
-        <v>302</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>383</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="L5" s="4" t="s">
+      <c r="J8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="4" t="s">
-        <v>342</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>343</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="L8" s="30"/>
+      <c r="M8" s="27"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>347</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="L6" s="2" t="s">
+      <c r="J9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
-        <v>69</v>
+        <v>248</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>70</v>
+        <v>249</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>117</v>
+        <v>384</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>386</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>74</v>
+        <v>253</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>253</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="K11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="4" t="s">
+        <v>342</v>
+      </c>
       <c r="C12" s="4" t="s">
-        <v>58</v>
+        <v>343</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>48</v>
+        <v>346</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>344</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>265</v>
+        <v>276</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>266</v>
+        <v>302</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L12" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="K16" s="32" t="s">
         <v>65</v>
-      </c>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="I14" s="34" t="s">
-        <v>112</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="N14" s="6"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:14">
       <c r="A17" s="4" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>405</v>
+        <v>354</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>195</v>
+        <v>302</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>401</v>
+        <v>355</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>411</v>
+        <v>276</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>348</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="L17" s="32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="31" customHeight="1">
+      <c r="A18" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K19" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="31" customHeight="1">
-      <c r="A18" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="G18" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="J18" s="29" t="s">
-        <v>253</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M18" s="30"/>
-      <c r="N18" s="27"/>
-    </row>
-    <row r="19" spans="1:14">
-      <c r="A19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="4"/>
-    </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="4" t="s">
-        <v>397</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1"/>
       <c r="C20" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>384</v>
+        <v>48</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>265</v>
+        <v>62</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H20" s="4" t="s">
-        <v>391</v>
+        <v>48</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>53</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K20" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="L20" s="32" t="s">
-        <v>57</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="4" t="s">
-        <v>58</v>
+        <v>287</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>176</v>
+        <v>288</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>186</v>
+        <v>290</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>182</v>
+        <v>289</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="32" t="s">
-        <v>181</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>291</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" s="27" customFormat="1" ht="55" customHeight="1">
+      <c r="A25" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="K25" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="A22" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>325</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="F23" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="I23" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="A24" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="L24" s="32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="27" customFormat="1" ht="55" customHeight="1">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I25" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="J25" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>57</v>
-      </c>
+      <c r="L25"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="4" t="s">
-        <v>348</v>
+      <c r="A26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>139</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>302</v>
+        <v>132</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>352</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>353</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>302</v>
+        <v>89</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="H26" s="36" t="s">
+        <v>135</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="L26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="1" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>248</v>
+        <v>274</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>249</v>
+        <v>42</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>148</v>
+        <v>275</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="I27" s="32" t="s">
-        <v>252</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>273</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="5"/>
       <c r="C28" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="D28" s="16" t="s">
-        <v>302</v>
+        <v>191</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>381</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>382</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="J28" s="16" t="s">
-        <v>383</v>
+        <v>194</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:14">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>144</v>
+        <v>208</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>146</v>
+        <v>209</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>142</v>
+        <v>210</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I29" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>57</v>
+        <v>207</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>287</v>
+        <v>217</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>288</v>
+        <v>153</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>290</v>
+        <v>218</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>291</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M30" s="4"/>
+        <v>216</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="31" spans="1:14">
-      <c r="A31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="1"/>
+      <c r="A31" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="C31" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>270</v>
+        <v>293</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>294</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>282</v>
+        <v>296</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>42</v>
+        <v>422</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I31" s="32" t="s">
-        <v>42</v>
+        <v>298</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M31" s="4"/>
+        <v>167</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:14">
       <c r="A32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>280</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="I32" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="I32" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M32" s="4"/>
-    </row>
-    <row r="33" spans="1:13">
-      <c r="A33" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>217</v>
+        <v>283</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>153</v>
+        <v>42</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>216</v>
-      </c>
-      <c r="I33" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13">
+        <v>284</v>
+      </c>
+      <c r="H33" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -8671,447 +8611,405 @@
       <c r="C34" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>261</v>
+      <c r="E34" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>153</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H34" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="I34" s="32" t="s">
+      <c r="H34" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K34" s="1" t="s">
+      <c r="J34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="M34" s="4"/>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="E35" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="G35" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="F35" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="I35" s="32" t="s">
+      <c r="H35" s="32" t="s">
         <v>162</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="K35" s="1" t="s">
+      <c r="J35" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L35" s="4" t="s">
+      <c r="K35" s="4" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
-      <c r="A36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="2"/>
+    <row r="36" spans="1:14">
+      <c r="A36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1"/>
       <c r="C36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>157</v>
+        <v>237</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I36" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+        <v>239</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H36" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>138</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B37" s="1"/>
       <c r="C37" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>279</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="G37" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="I37" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="4" t="s">
-        <v>335</v>
-      </c>
+        <v>223</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="H37" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1"/>
       <c r="C38" s="4" t="s">
-        <v>302</v>
+        <v>118</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>248</v>
+        <v>119</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>265</v>
+        <v>121</v>
       </c>
       <c r="G38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="H38" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13">
+      <c r="J38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>239</v>
+        <v>230</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="I39" s="32" t="s">
-        <v>240</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M39" s="4"/>
-    </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>139</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1"/>
       <c r="C40" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>304</v>
+        <v>230</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>305</v>
+        <v>231</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>302</v>
+        <v>69</v>
+      </c>
+      <c r="H40" s="32" t="s">
+        <v>232</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>298</v>
+        <v>54</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="L40" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:13">
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="4" t="s">
-        <v>207</v>
+        <v>70</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>209</v>
+        <v>117</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="I41" s="32" t="s">
-        <v>213</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="K41" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13">
+        <v>69</v>
+      </c>
+      <c r="H41" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="4" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>277</v>
+        <v>117</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>154</v>
+        <v>71</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="H42" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I42" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="J42" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="K42" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L42" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13">
+        <v>73</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G43" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I43" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="K43" s="1" t="s">
+      <c r="H43" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L43" s="4"/>
+      <c r="N43" s="27"/>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="L43" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13">
-      <c r="A44" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="4" t="s">
-        <v>222</v>
+        <v>70</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>223</v>
+        <v>109</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="I44" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="K44" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L44" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M44" s="4"/>
-    </row>
-    <row r="45" spans="1:13">
-      <c r="A45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>42</v>
+        <v>69</v>
+      </c>
+      <c r="H44" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>382</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>275</v>
+        <v>380</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="I45" s="32" t="s">
-        <v>49</v>
+        <v>377</v>
+      </c>
+      <c r="I45" s="16" t="s">
+        <v>383</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L45" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M45" s="4"/>
-    </row>
-    <row r="50" spans="1:14">
+        <v>324</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="J50"/>
       <c r="K50"/>
-      <c r="L50"/>
-    </row>
-    <row r="51" spans="1:14">
-      <c r="A51" s="9" t="s">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="9"/>
       <c r="B51" s="9"/>
-      <c r="C51" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F51" s="9"/>
-      <c r="G51" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>59</v>
-      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
       <c r="I51" s="9"/>
-      <c r="J51" s="9"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="9"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:N51">
-    <sortCondition ref="I2:I51"/>
-    <sortCondition ref="J2:J51"/>
+    <sortCondition ref="G2:G51"/>
+    <sortCondition ref="H2:H51"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Clarifying key points in paper
</commit_message>
<xml_diff>
--- a/conceptual paper/study summary.xlsx
+++ b/conceptual paper/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20740" yWindow="2040" windowWidth="24960" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="26320" yWindow="1840" windowWidth="24960" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all studies" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1588" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="431">
   <si>
     <t>define match</t>
   </si>
@@ -914,6 +914,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t>(peak biomass)</t>
@@ -935,6 +936,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="128"/>
         <scheme val="minor"/>
       </rPr>
       <t>(density)</t>
@@ -1353,6 +1355,15 @@
   </si>
   <si>
     <t>Senner, N.R., Stager, M. and Sandercock, B.K., 2017. Ecological mismatches are moderated by local conditions for two populations of a long‐distance migratory bird. Oikos, 126(1), pp.61-72.</t>
+  </si>
+  <si>
+    <t>Reneerkens J, Schmidt NM, Gilg O, Hansen J, Holst Hansen L, et al. 2016. Effects of food abundance and</t>
+  </si>
+  <si>
+    <t>early clutch predation on reproductive timing in a high Arctic shorebird exposed to advancements in</t>
+  </si>
+  <si>
+    <t>arthropod abundance. Ecol. Evol. 6:7375–86</t>
   </si>
 </sst>
 </file>
@@ -1365,6 +1376,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3358,11 +3370,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q40"/>
+  <dimension ref="A1:Q44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3852,44 +3864,59 @@
         <v>373</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>427</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="B42" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="B43" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" t="s">
+        <v>430</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisions on ms version 4
</commit_message>
<xml_diff>
--- a/conceptual paper/study summary.xlsx
+++ b/conceptual paper/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26320" yWindow="1840" windowWidth="24960" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="all studies" sheetId="4" r:id="rId1"/>
@@ -3372,7 +3372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
     </sheetView>
@@ -7542,9 +7542,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7555,7 +7555,7 @@
     <col min="4" max="4" width="18.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="4" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18" style="4" customWidth="1"/>
+    <col min="7" max="7" width="27.5" style="4" customWidth="1"/>
     <col min="8" max="8" width="26.6640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="19.1640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="8.33203125" style="4" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
tweak to appendix, updates to study database
</commit_message>
<xml_diff>
--- a/conceptual paper/study summary.xlsx
+++ b/conceptual paper/study summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="30000" yWindow="0" windowWidth="25600" windowHeight="20120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="all studies" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1616" uniqueCount="439">
   <si>
     <t>define match</t>
   </si>
@@ -1345,9 +1345,6 @@
     <t>(5) Saino, N., Ambrosini, R., Rubolini, D., von Hardenberg, J., Provenzale, A., Huppop, K. et al. (2011) Climate warming, ecological mismatch at arrival and population decline in migratory birds. Proceedings of the Royal Society of London B, 278, 835–842.’’</t>
   </si>
   <si>
-    <t>(6) Samplonius, J.M., Kappers, E.F., Brands, S. and Both, C., 2016. Phenological mismatch and ontogenetic diet shifts interactively affect offspring condition in a passerine. Journal of Animal Ecology, 85(5), pp.1255-1264.</t>
-  </si>
-  <si>
     <t>(7) Knell, R.J. and Thackeray, S.J., 2016. Voltinism and resilience to climate-induced phenological mismatch. Climatic change, 137(3-4), pp.525-539.</t>
   </si>
   <si>
@@ -1364,6 +1361,33 @@
   </si>
   <si>
     <t>arthropod abundance. Ecol. Evol. 6:7375–86</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>HMK070</t>
+  </si>
+  <si>
+    <t>1954, 2005-2008</t>
+  </si>
+  <si>
+    <t>visser et al. 2006</t>
+  </si>
+  <si>
+    <t>arctic arthropods is their main food resource</t>
+  </si>
+  <si>
+    <t>arthropod (many spp, resolved to family level)</t>
+  </si>
+  <si>
+    <t>individual (chick growth)</t>
+  </si>
+  <si>
+    <t>HMK033</t>
+  </si>
+  <si>
+    <t>performance not measured in observational part of study, only experimental</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1521,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="689">
+  <cellStyleXfs count="755">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2187,8 +2211,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2351,8 +2441,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="689">
+  <cellStyles count="755">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2697,6 +2788,39 @@
     <cellStyle name="Followed Hyperlink" xfId="684" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3041,6 +3165,39 @@
     <cellStyle name="Hyperlink" xfId="683" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3370,11 +3527,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q44"/>
+  <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3422,172 +3579,163 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="6"/>
+      <c r="A2" s="60" t="s">
+        <v>430</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>256</v>
-      </c>
-      <c r="B3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" s="4"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="60"/>
+      <c r="B4" s="60"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>256</v>
       </c>
       <c r="B5" t="s">
-        <v>258</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>187</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="L5" s="19" t="s">
-        <v>188</v>
-      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>259</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="L6" s="9" t="s">
-        <v>100</v>
-      </c>
+        <v>256</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>256</v>
       </c>
       <c r="B7" t="s">
-        <v>378</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="24" t="s">
-        <v>166</v>
+        <v>258</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="L7" s="19" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>256</v>
-      </c>
-      <c r="B8" t="s">
-        <v>323</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="D8" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>322</v>
+      <c r="E8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
+      <c r="I8" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>256</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>331</v>
+      <c r="B9" t="s">
+        <v>378</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>165</v>
       </c>
       <c r="D9" s="24"/>
       <c r="E9" s="9"/>
@@ -3597,61 +3745,87 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="24" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>256</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="B10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>322</v>
+      </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>387</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>338</v>
-      </c>
+      <c r="B11" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="D11" s="24"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>256</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>333</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+        <v>332</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>256</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>390</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>334</v>
+      <c r="B13" s="24" t="s">
+        <v>387</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -3659,130 +3833,56 @@
         <v>256</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>340</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>256</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>414</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>341</v>
+        <v>390</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>256</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>415</v>
+      <c r="B16" s="17" t="s">
+        <v>330</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>256</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>364</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>363</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="O17" s="4" t="s">
-        <v>365</v>
-      </c>
-      <c r="P17" s="4" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q17" s="4" t="s">
-        <v>367</v>
+      <c r="B17" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:17">
       <c r="A18" t="s">
         <v>256</v>
       </c>
-      <c r="B18" s="34" t="s">
-        <v>313</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="Q18" s="4" t="s">
-        <v>377</v>
+      <c r="B18" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -3790,133 +3890,231 @@
         <v>256</v>
       </c>
       <c r="B19" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="P20" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q20" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="34" t="s">
+      <c r="C21" s="34" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24" t="s">
-        <v>416</v>
-      </c>
-      <c r="C20" s="34" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="A21" s="24"/>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="24"/>
+      <c r="B22" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="23" spans="1:17">
-      <c r="A23" s="34"/>
+      <c r="A23" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>323</v>
+      </c>
+      <c r="C23" t="s">
+        <v>370</v>
+      </c>
     </row>
     <row r="24" spans="1:17">
-      <c r="A24" s="24" t="s">
+      <c r="A24" t="s">
+        <v>256</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C24" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="s">
+        <v>256</v>
+      </c>
+      <c r="B25" t="s">
+        <v>323</v>
+      </c>
+      <c r="C25" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" s="24" t="s">
         <v>357</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B26" s="24" t="s">
         <v>358</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C26" s="34" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24" t="s">
+    <row r="27" spans="1:17">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24" t="s">
         <v>360</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C27" s="34" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
-      <c r="A26" s="24"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="34"/>
-    </row>
-    <row r="27" spans="1:17">
-      <c r="A27" s="34"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="34"/>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="A29" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17">
-      <c r="A30" s="17" t="s">
-        <v>369</v>
+    <row r="28" spans="1:17">
+      <c r="A28" s="60" t="s">
+        <v>256</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>438</v>
+      </c>
+      <c r="C28" s="60" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17">
-      <c r="A32" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>394</v>
+        <v>368</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>423</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" t="s">
-        <v>426</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>427</v>
+        <v>424</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="B42" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
-      <c r="B43" t="s">
-        <v>429</v>
+      <c r="A42" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="B44" t="s">
-        <v>430</v>
+        <v>427</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="B45" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="B46" t="s">
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -3932,11 +4130,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4837,50 +5035,73 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="2"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2"/>
-      <c r="B43" s="25"/>
+      <c r="B43" s="32"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="2"/>
+      <c r="B44" s="25"/>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B45" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D45" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9" t="s">
+      <c r="E45" s="9"/>
+      <c r="F45" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9" t="s">
+      <c r="G45" s="9"/>
+      <c r="H45" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="I44" s="9" t="s">
+      <c r="I45" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50"/>
-      <c r="B50"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
+    <row r="46" spans="1:9">
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4898,10 +5119,10 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6197,6 +6418,32 @@
       </c>
       <c r="I45" s="4" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="51" spans="1:13">
@@ -6305,7 +6552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView topLeftCell="D5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -7542,8 +7789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>

</xml_diff>